<commit_message>
Few changes on Tableau
</commit_message>
<xml_diff>
--- a/DATABASE RESTAURANT MADE BY ME/excels/Restaurante.xlsx
+++ b/DATABASE RESTAURANT MADE BY ME/excels/Restaurante.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victormorenorequena/Desktop/BASE DE DATOS MORENO/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victormorenorequena/Desktop/My_Projects/DATABASE RESTAURANT MADE BY ME/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A929295F-BEED-B541-98C4-5D48FC0B2FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580BE7A0-4639-524E-A116-5379C403A51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="4" xr2:uid="{54D0E52C-6CE4-7B45-A605-5927E0CE42E7}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{54D0E52C-6CE4-7B45-A605-5927E0CE42E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Ventas" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="1272">
   <si>
     <t>Venta_ID</t>
   </si>
@@ -3823,9 +3823,6 @@
   </si>
   <si>
     <t>Emilio Moro malleolus</t>
-  </si>
-  <si>
-    <t>Vino_I+A1:B2D</t>
   </si>
   <si>
     <t>Tienda</t>
@@ -30392,8 +30389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550F48B7-5A57-7845-8656-5FA00F9726C3}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30405,7 +30402,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>1261</v>
+        <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1143</v>
@@ -31076,7 +31073,7 @@
         <v>1171</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" ref="F3:F66" si="4">D21-C21</f>
+        <f t="shared" ref="F21:F66" si="4">D21-C21</f>
         <v>36</v>
       </c>
       <c r="G21" s="7" t="e">
@@ -33559,7 +33556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C804708-3991-C745-99A1-613DAA0130DF}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
@@ -33570,19 +33567,19 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C1" t="s">
         <v>1262</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1263</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1264</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1265</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1266</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -33590,16 +33587,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C2" t="s">
         <v>1267</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1268</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1269</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1270</v>
       </c>
       <c r="F2">
         <v>17</v>
@@ -33610,16 +33607,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E3" t="s">
         <v>1271</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1268</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1272</v>
       </c>
       <c r="F3">
         <v>8</v>

</xml_diff>